<commit_message>
Update DRV, KGE and R2s documents
</commit_message>
<xml_diff>
--- a/docs/_static/notes/general_table.xlsx
+++ b/docs/_static/notes/general_table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\libs\permetrics\docs\_static\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{D4CEF450-1CF8-4870-8446-170873DE471B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953B95FE-B9BC-4B39-A349-3B9CB8E51FD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Problem</t>
   </si>
@@ -165,12 +165,30 @@
   </si>
   <si>
     <t>Smaller is better (Best = 0)</t>
+  </si>
+  <si>
+    <t>R2s</t>
+  </si>
+  <si>
+    <t>DRV</t>
+  </si>
+  <si>
+    <t>KGE</t>
+  </si>
+  <si>
+    <t>(Pearson’s Correlation Index) ^ 2</t>
+  </si>
+  <si>
+    <t>Deviation of Runoff Volume</t>
+  </si>
+  <si>
+    <t>Kling-Gupta Efficiency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -264,11 +282,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFE2E5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -289,6 +318,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -604,11 +639,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,7 +915,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1">
         <v>17</v>
       </c>
@@ -895,30 +930,75 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B22" s="5">
         <v>1</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B23" s="5">
         <v>1</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A2:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>